<commit_message>
Change Golem => Bear
</commit_message>
<xml_diff>
--- a/Monster_stat.xlsx
+++ b/Monster_stat.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
-    <t>Golem</t>
-  </si>
-  <si>
     <t>Wolf</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Bear</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,42 +783,42 @@
       <c r="A3" s="1"/>
       <c r="B3" s="22"/>
       <c r="C3" s="32" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" s="29"/>
       <c r="K3" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L3" s="28"/>
       <c r="M3" s="2"/>
       <c r="N3" s="1"/>
       <c r="O3" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T3" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -829,52 +829,52 @@
       <c r="A4" s="1"/>
       <c r="B4" s="23"/>
       <c r="C4" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="1"/>
       <c r="O4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R4" s="14"/>
       <c r="S4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -884,48 +884,48 @@
     <row r="5" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="1"/>
       <c r="O5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -934,42 +934,42 @@
     <row r="6" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="1"/>
       <c r="O6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -978,42 +978,42 @@
     <row r="7" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="1"/>
       <c r="O7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1022,44 +1022,44 @@
     <row r="8" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="1"/>
       <c r="O8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
@@ -1068,42 +1068,42 @@
     <row r="9" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -1112,33 +1112,33 @@
     <row r="10" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1151,26 +1151,26 @@
     <row r="11" spans="1:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L11" s="21"/>
       <c r="M11" s="1"/>

</xml_diff>